<commit_message>
Data files as of 2018-12-03
Data files as of 2018-12-03 Test Cases Pl.xlsx file.
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases Pl.xlsx
+++ b/src/com/data/Test Cases Pl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="22260" windowHeight="10200" tabRatio="152" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="18300" windowHeight="5880" tabRatio="152" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7622" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7622" uniqueCount="307">
   <si>
     <t>TCID</t>
   </si>
@@ -934,6 +934,9 @@
   </si>
   <si>
     <t>Standard Plan Examination or Review</t>
+  </si>
+  <si>
+    <t>1 :: Electrical Motors :: DOBTESTING123@GMAIL.COM :: Professional Engineer</t>
   </si>
 </sst>
 </file>
@@ -2782,9 +2785,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -13809,7 +13812,7 @@
         <v>159</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>4</v>
+        <v>163</v>
       </c>
       <c r="H97" s="5" t="s">
         <v>249</v>
@@ -17306,7 +17309,7 @@
         <v>159</v>
       </c>
       <c r="G125" s="5" t="s">
-        <v>4</v>
+        <v>163</v>
       </c>
       <c r="H125" s="5" t="s">
         <v>242</v>
@@ -17350,7 +17353,7 @@
         <v>280</v>
       </c>
       <c r="W125" s="12" t="s">
-        <v>213</v>
+        <v>306</v>
       </c>
       <c r="X125" s="12"/>
       <c r="Y125" s="12"/>
@@ -19603,10 +19606,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:93">
+    <row r="144" spans="1:93" ht="409.6">
       <c r="E144" s="30"/>
     </row>
-    <row r="145" spans="1:93" s="8" customFormat="1">
+    <row r="145" spans="1:93" s="8" customFormat="1" ht="409.6">
       <c r="A145" s="37" t="s">
         <v>246</v>
       </c>
@@ -20109,10 +20112,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:93">
+    <row r="148" spans="1:93" ht="409.6">
       <c r="E148" s="30"/>
     </row>
-    <row r="149" spans="1:93" s="8" customFormat="1">
+    <row r="149" spans="1:93" s="8" customFormat="1" ht="409.6">
       <c r="A149" s="37" t="s">
         <v>178</v>
       </c>
@@ -20615,10 +20618,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:93">
+    <row r="152" spans="1:93" ht="409.6">
       <c r="E152" s="30"/>
     </row>
-    <row r="153" spans="1:93" s="8" customFormat="1">
+    <row r="153" spans="1:93" s="8" customFormat="1" ht="409.6">
       <c r="A153" s="37" t="s">
         <v>203</v>
       </c>
@@ -21121,10 +21124,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:93">
+    <row r="156" spans="1:93" ht="409.6">
       <c r="E156" s="30"/>
     </row>
-    <row r="157" spans="1:93" s="8" customFormat="1">
+    <row r="157" spans="1:93" s="8" customFormat="1" ht="409.6">
       <c r="A157" s="37" t="s">
         <v>185</v>
       </c>
@@ -21627,10 +21630,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:93">
+    <row r="160" spans="1:93" ht="409.6">
       <c r="E160" s="30"/>
     </row>
-    <row r="161" spans="1:93" s="8" customFormat="1">
+    <row r="161" spans="1:93" s="8" customFormat="1" ht="409.6">
       <c r="A161" s="37" t="s">
         <v>209</v>
       </c>
@@ -22133,10 +22136,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:93">
+    <row r="164" spans="1:93" ht="409.6">
       <c r="E164" s="30"/>
     </row>
-    <row r="165" spans="1:93" s="8" customFormat="1">
+    <row r="165" spans="1:93" s="8" customFormat="1" ht="409.6">
       <c r="A165" s="37" t="s">
         <v>179</v>
       </c>

</xml_diff>

<commit_message>
Data files as of 2018-12-04
Data file Test Cases.PL.xlsx as of 2018-12-04
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases Pl.xlsx
+++ b/src/com/data/Test Cases Pl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="18300" windowHeight="5880" tabRatio="152" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="18300" windowHeight="10200" tabRatio="152" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -2785,9 +2785,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F97" sqref="F97"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W97" sqref="W97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -13856,7 +13856,7 @@
         <v>280</v>
       </c>
       <c r="W97" s="12" t="s">
-        <v>213</v>
+        <v>306</v>
       </c>
       <c r="X97" s="12"/>
       <c r="Y97" s="12"/>
@@ -19606,10 +19606,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:93" ht="409.6">
+    <row r="144" spans="1:93">
       <c r="E144" s="30"/>
     </row>
-    <row r="145" spans="1:93" s="8" customFormat="1" ht="409.6">
+    <row r="145" spans="1:93" s="8" customFormat="1">
       <c r="A145" s="37" t="s">
         <v>246</v>
       </c>
@@ -20112,10 +20112,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:93" ht="409.6">
+    <row r="148" spans="1:93">
       <c r="E148" s="30"/>
     </row>
-    <row r="149" spans="1:93" s="8" customFormat="1" ht="409.6">
+    <row r="149" spans="1:93" s="8" customFormat="1">
       <c r="A149" s="37" t="s">
         <v>178</v>
       </c>
@@ -20618,10 +20618,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:93" ht="409.6">
+    <row r="152" spans="1:93">
       <c r="E152" s="30"/>
     </row>
-    <row r="153" spans="1:93" s="8" customFormat="1" ht="409.6">
+    <row r="153" spans="1:93" s="8" customFormat="1">
       <c r="A153" s="37" t="s">
         <v>203</v>
       </c>
@@ -21124,10 +21124,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:93" ht="409.6">
+    <row r="156" spans="1:93">
       <c r="E156" s="30"/>
     </row>
-    <row r="157" spans="1:93" s="8" customFormat="1" ht="409.6">
+    <row r="157" spans="1:93" s="8" customFormat="1">
       <c r="A157" s="37" t="s">
         <v>185</v>
       </c>
@@ -21630,10 +21630,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:93" ht="409.6">
+    <row r="160" spans="1:93">
       <c r="E160" s="30"/>
     </row>
-    <row r="161" spans="1:93" s="8" customFormat="1" ht="409.6">
+    <row r="161" spans="1:93" s="8" customFormat="1">
       <c r="A161" s="37" t="s">
         <v>209</v>
       </c>
@@ -22136,10 +22136,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:93" ht="409.6">
+    <row r="164" spans="1:93">
       <c r="E164" s="30"/>
     </row>
-    <row r="165" spans="1:93" s="8" customFormat="1" ht="409.6">
+    <row r="165" spans="1:93" s="8" customFormat="1">
       <c r="A165" s="37" t="s">
         <v>179</v>
       </c>
@@ -22642,10 +22642,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:93" ht="409.6">
+    <row r="168" spans="1:93">
       <c r="E168" s="30"/>
     </row>
-    <row r="169" spans="1:93" s="8" customFormat="1" ht="409.6">
+    <row r="169" spans="1:93" s="8" customFormat="1">
       <c r="A169" s="37" t="s">
         <v>207</v>
       </c>
@@ -23148,7 +23148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:93" ht="409.6">
+    <row r="172" spans="1:93">
       <c r="E172" s="30"/>
     </row>
     <row r="173" spans="1:93" s="8" customFormat="1" ht="409.6">

</xml_diff>

<commit_message>
latest data files as of 2018-12-12 PM
latest data files as of 2018-12-12 PM - test cases incl. MsNew
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases Pl.xlsx
+++ b/src/com/data/Test Cases Pl.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="23475" windowHeight="10110" tabRatio="152" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="23475" windowHeight="10200" tabRatio="152" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A128:J146"/>
+  <oleSize ref="A126:K145"/>
 </workbook>
 </file>
 
@@ -954,9 +954,6 @@
     <t>Structural :: 1111 :: 1.00 :: 3333</t>
   </si>
   <si>
-    <t>MhNew</t>
-  </si>
-  <si>
     <t>Mechanical Systems - New</t>
   </si>
   <si>
@@ -994,6 +991,9 @@
   </si>
   <si>
     <t>NYCECC :: Tabular Analysis :: Y</t>
+  </si>
+  <si>
+    <t>MsNew</t>
   </si>
 </sst>
 </file>
@@ -2218,8 +2218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="12.75"/>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="37" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="C75" s="33" t="s">
         <v>3</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="37" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C76" s="33" t="s">
         <v>3</v>
@@ -2855,9 +2855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L134" sqref="L134"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -3533,7 +3533,7 @@
         <v>108</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M6" s="12" t="s">
         <v>165</v>
@@ -4864,7 +4864,7 @@
         <v>108</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M25" s="12" t="s">
         <v>165</v>
@@ -5367,7 +5367,7 @@
         <v>108</v>
       </c>
       <c r="L29" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M29" s="12" t="s">
         <v>165</v>
@@ -5870,7 +5870,7 @@
         <v>108</v>
       </c>
       <c r="L33" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M33" s="12" t="s">
         <v>165</v>
@@ -6373,7 +6373,7 @@
         <v>108</v>
       </c>
       <c r="L37" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M37" s="12" t="s">
         <v>165</v>
@@ -6879,7 +6879,7 @@
         <v>108</v>
       </c>
       <c r="L41" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M41" s="12" t="s">
         <v>165</v>
@@ -7386,7 +7386,7 @@
         <v>108</v>
       </c>
       <c r="L45" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M45" s="12" t="s">
         <v>165</v>
@@ -7890,7 +7890,7 @@
         <v>108</v>
       </c>
       <c r="L49" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M49" s="12" t="s">
         <v>165</v>
@@ -8400,7 +8400,7 @@
         <v>108</v>
       </c>
       <c r="L53" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M53" s="12" t="s">
         <v>165</v>
@@ -8859,7 +8859,7 @@
         <v>108</v>
       </c>
       <c r="L57" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M57" s="12" t="s">
         <v>165</v>
@@ -9366,7 +9366,7 @@
         <v>108</v>
       </c>
       <c r="L61" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M61" s="12" t="s">
         <v>165</v>
@@ -9873,7 +9873,7 @@
         <v>108</v>
       </c>
       <c r="L65" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M65" s="12" t="s">
         <v>165</v>
@@ -10376,7 +10376,7 @@
         <v>108</v>
       </c>
       <c r="L69" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M69" s="12" t="s">
         <v>165</v>
@@ -10879,7 +10879,7 @@
         <v>108</v>
       </c>
       <c r="L73" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M73" s="12" t="s">
         <v>165</v>
@@ -11382,7 +11382,7 @@
         <v>108</v>
       </c>
       <c r="L77" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M77" s="12" t="s">
         <v>165</v>
@@ -11885,7 +11885,7 @@
         <v>108</v>
       </c>
       <c r="L81" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M81" s="12" t="s">
         <v>165</v>
@@ -12388,7 +12388,7 @@
         <v>108</v>
       </c>
       <c r="L85" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M85" s="12" t="s">
         <v>165</v>
@@ -12891,7 +12891,7 @@
         <v>108</v>
       </c>
       <c r="L89" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M89" s="12" t="s">
         <v>165</v>
@@ -13394,7 +13394,7 @@
         <v>108</v>
       </c>
       <c r="L93" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M93" s="12" t="s">
         <v>165</v>
@@ -13948,7 +13948,7 @@
         <v>108</v>
       </c>
       <c r="L97" s="12" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="M97" s="12" t="s">
         <v>165</v>
@@ -13974,7 +13974,7 @@
         <v>138</v>
       </c>
       <c r="V97" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="W97" s="12" t="s">
         <v>305</v>
@@ -14502,7 +14502,7 @@
         <v>108</v>
       </c>
       <c r="L101" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M101" s="12" t="s">
         <v>165</v>
@@ -15005,7 +15005,7 @@
         <v>108</v>
       </c>
       <c r="L105" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M105" s="12" t="s">
         <v>165</v>
@@ -15502,7 +15502,7 @@
         <v>108</v>
       </c>
       <c r="L109" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M109" s="12" t="s">
         <v>165</v>
@@ -15999,7 +15999,7 @@
         <v>108</v>
       </c>
       <c r="L113" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M113" s="12" t="s">
         <v>165</v>
@@ -16499,7 +16499,7 @@
         <v>108</v>
       </c>
       <c r="L117" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M117" s="12" t="s">
         <v>165</v>
@@ -16999,7 +16999,7 @@
         <v>108</v>
       </c>
       <c r="L121" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M121" s="12" t="s">
         <v>165</v>
@@ -17496,7 +17496,7 @@
         <v>108</v>
       </c>
       <c r="L125" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M125" s="12" t="s">
         <v>165</v>
@@ -17522,7 +17522,7 @@
         <v>122</v>
       </c>
       <c r="V125" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="W125" s="12" t="s">
         <v>305</v>
@@ -17993,7 +17993,7 @@
         <v>108</v>
       </c>
       <c r="L129" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M129" s="12" t="s">
         <v>165</v>
@@ -18541,7 +18541,7 @@
         <v>309</v>
       </c>
       <c r="L133" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M133" s="12" t="s">
         <v>165</v>
@@ -18732,7 +18732,7 @@
     </row>
     <row r="135" spans="1:102" s="8" customFormat="1">
       <c r="A135" s="37" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="B135" s="7"/>
       <c r="E135" s="7"/>
@@ -19065,7 +19065,7 @@
         <v>3</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C137" s="21" t="s">
         <v>304</v>
@@ -19074,7 +19074,7 @@
         <v>221</v>
       </c>
       <c r="E137" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F137" s="5" t="s">
         <v>158</v>
@@ -19095,7 +19095,7 @@
         <v>309</v>
       </c>
       <c r="L137" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M137" s="12" t="s">
         <v>165</v>
@@ -19118,13 +19118,13 @@
         <v>139</v>
       </c>
       <c r="U137" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="V137" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="V137" s="5" t="s">
+      <c r="W137" s="12" t="s">
         <v>316</v>
-      </c>
-      <c r="W137" s="12" t="s">
-        <v>317</v>
       </c>
       <c r="X137" s="12"/>
       <c r="Y137" s="12"/>
@@ -19286,7 +19286,7 @@
     </row>
     <row r="139" spans="1:102" s="8" customFormat="1">
       <c r="A139" s="37" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B139" s="7"/>
       <c r="E139" s="7"/>
@@ -19619,7 +19619,7 @@
         <v>3</v>
       </c>
       <c r="B141" s="22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C141" s="21" t="s">
         <v>304</v>
@@ -19628,7 +19628,7 @@
         <v>221</v>
       </c>
       <c r="E141" s="19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F141" s="5" t="s">
         <v>158</v>
@@ -19649,7 +19649,7 @@
         <v>309</v>
       </c>
       <c r="L141" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M141" s="12" t="s">
         <v>165</v>
@@ -19672,13 +19672,13 @@
         <v>139</v>
       </c>
       <c r="U141" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="V141" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="W141" s="12" t="s">
         <v>321</v>
-      </c>
-      <c r="V141" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="W141" s="12" t="s">
-        <v>322</v>
       </c>
       <c r="X141" s="12"/>
       <c r="Y141" s="12"/>
@@ -20479,7 +20479,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:102" s="11" customFormat="1">
+    <row r="148" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A148" s="10"/>
       <c r="B148" s="18"/>
       <c r="E148" s="30"/>
@@ -20530,7 +20530,7 @@
       <c r="BP148" s="10"/>
       <c r="BQ148" s="10"/>
     </row>
-    <row r="149" spans="1:102" s="8" customFormat="1">
+    <row r="149" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A149" s="37" t="s">
         <v>244</v>
       </c>
@@ -21033,7 +21033,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:102" s="11" customFormat="1">
+    <row r="152" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A152" s="10"/>
       <c r="B152" s="18"/>
       <c r="E152" s="30"/>
@@ -21084,7 +21084,7 @@
       <c r="BP152" s="10"/>
       <c r="BQ152" s="10"/>
     </row>
-    <row r="153" spans="1:102" s="8" customFormat="1">
+    <row r="153" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A153" s="37" t="s">
         <v>191</v>
       </c>
@@ -21587,7 +21587,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:102" s="11" customFormat="1">
+    <row r="156" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A156" s="10"/>
       <c r="B156" s="18"/>
       <c r="E156" s="30"/>
@@ -21638,7 +21638,7 @@
       <c r="BP156" s="10"/>
       <c r="BQ156" s="10"/>
     </row>
-    <row r="157" spans="1:102" s="8" customFormat="1">
+    <row r="157" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A157" s="37" t="s">
         <v>245</v>
       </c>
@@ -22141,7 +22141,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:102" s="11" customFormat="1">
+    <row r="160" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A160" s="10"/>
       <c r="B160" s="18"/>
       <c r="E160" s="30"/>
@@ -22192,7 +22192,7 @@
       <c r="BP160" s="10"/>
       <c r="BQ160" s="10"/>
     </row>
-    <row r="161" spans="1:102" s="8" customFormat="1">
+    <row r="161" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A161" s="37" t="s">
         <v>177</v>
       </c>
@@ -22695,7 +22695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:102" s="11" customFormat="1">
+    <row r="164" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A164" s="10"/>
       <c r="B164" s="18"/>
       <c r="E164" s="30"/>
@@ -22746,7 +22746,7 @@
       <c r="BP164" s="10"/>
       <c r="BQ164" s="10"/>
     </row>
-    <row r="165" spans="1:102" s="8" customFormat="1">
+    <row r="165" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A165" s="37" t="s">
         <v>202</v>
       </c>
@@ -23249,7 +23249,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:102" s="11" customFormat="1">
+    <row r="168" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A168" s="10"/>
       <c r="B168" s="18"/>
       <c r="E168" s="30"/>
@@ -23300,7 +23300,7 @@
       <c r="BP168" s="10"/>
       <c r="BQ168" s="10"/>
     </row>
-    <row r="169" spans="1:102" s="8" customFormat="1">
+    <row r="169" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A169" s="37" t="s">
         <v>184</v>
       </c>
@@ -23803,7 +23803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:102" s="11" customFormat="1">
+    <row r="172" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A172" s="10"/>
       <c r="B172" s="18"/>
       <c r="E172" s="30"/>
@@ -23854,7 +23854,7 @@
       <c r="BP172" s="10"/>
       <c r="BQ172" s="10"/>
     </row>
-    <row r="173" spans="1:102" s="8" customFormat="1">
+    <row r="173" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A173" s="37" t="s">
         <v>208</v>
       </c>
@@ -24357,7 +24357,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="1:102" s="11" customFormat="1">
+    <row r="176" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A176" s="10"/>
       <c r="B176" s="18"/>
       <c r="E176" s="30"/>
@@ -24408,7 +24408,7 @@
       <c r="BP176" s="10"/>
       <c r="BQ176" s="10"/>
     </row>
-    <row r="177" spans="1:102" s="8" customFormat="1">
+    <row r="177" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A177" s="37" t="s">
         <v>178</v>
       </c>
@@ -24911,7 +24911,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:102" s="11" customFormat="1">
+    <row r="180" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A180" s="10"/>
       <c r="B180" s="18"/>
       <c r="E180" s="30"/>
@@ -24962,7 +24962,7 @@
       <c r="BP180" s="10"/>
       <c r="BQ180" s="10"/>
     </row>
-    <row r="181" spans="1:102" s="8" customFormat="1">
+    <row r="181" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A181" s="37" t="s">
         <v>206</v>
       </c>
@@ -25465,7 +25465,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:102" s="11" customFormat="1">
+    <row r="184" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A184" s="10"/>
       <c r="B184" s="18"/>
       <c r="E184" s="30"/>
@@ -25516,7 +25516,7 @@
       <c r="BP184" s="10"/>
       <c r="BQ184" s="10"/>
     </row>
-    <row r="185" spans="1:102" s="8" customFormat="1">
+    <row r="185" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A185" s="37" t="s">
         <v>174</v>
       </c>
@@ -26019,7 +26019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="188" spans="1:102" s="11" customFormat="1">
+    <row r="188" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A188" s="10"/>
       <c r="B188" s="18"/>
       <c r="E188" s="30"/>
@@ -26070,7 +26070,7 @@
       <c r="BP188" s="10"/>
       <c r="BQ188" s="10"/>
     </row>
-    <row r="189" spans="1:102" s="8" customFormat="1">
+    <row r="189" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A189" s="37" t="s">
         <v>200</v>
       </c>
@@ -26573,7 +26573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="192" spans="1:102" s="11" customFormat="1">
+    <row r="192" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A192" s="10"/>
       <c r="B192" s="18"/>
       <c r="E192" s="30"/>
@@ -26624,7 +26624,7 @@
       <c r="BP192" s="10"/>
       <c r="BQ192" s="10"/>
     </row>
-    <row r="193" spans="1:102" s="8" customFormat="1">
+    <row r="193" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A193" s="37" t="s">
         <v>234</v>
       </c>
@@ -27127,7 +27127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:102" s="11" customFormat="1">
+    <row r="196" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A196" s="10"/>
       <c r="B196" s="18"/>
       <c r="E196" s="30"/>
@@ -27178,7 +27178,7 @@
       <c r="BP196" s="10"/>
       <c r="BQ196" s="10"/>
     </row>
-    <row r="197" spans="1:102" s="8" customFormat="1">
+    <row r="197" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A197" s="37" t="s">
         <v>236</v>
       </c>
@@ -27681,7 +27681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="200" spans="1:102" s="11" customFormat="1">
+    <row r="200" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A200" s="10"/>
       <c r="B200" s="18"/>
       <c r="E200" s="30"/>
@@ -27732,7 +27732,7 @@
       <c r="BP200" s="10"/>
       <c r="BQ200" s="10"/>
     </row>
-    <row r="201" spans="1:102" s="8" customFormat="1">
+    <row r="201" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A201" s="37" t="s">
         <v>232</v>
       </c>
@@ -28235,7 +28235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="204" spans="1:102" s="11" customFormat="1">
+    <row r="204" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A204" s="10"/>
       <c r="B204" s="18"/>
       <c r="E204" s="30"/>
@@ -28286,7 +28286,7 @@
       <c r="BP204" s="10"/>
       <c r="BQ204" s="10"/>
     </row>
-    <row r="205" spans="1:102" s="8" customFormat="1">
+    <row r="205" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A205" s="37" t="s">
         <v>238</v>
       </c>
@@ -28789,7 +28789,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:102" s="11" customFormat="1">
+    <row r="208" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A208" s="10"/>
       <c r="B208" s="18"/>
       <c r="E208" s="30"/>
@@ -28840,7 +28840,7 @@
       <c r="BP208" s="10"/>
       <c r="BQ208" s="10"/>
     </row>
-    <row r="209" spans="1:102" s="8" customFormat="1">
+    <row r="209" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A209" s="37" t="s">
         <v>171</v>
       </c>
@@ -29205,7 +29205,7 @@
         <v>163</v>
       </c>
       <c r="L211" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M211" s="12" t="s">
         <v>165</v>
@@ -29345,7 +29345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:102" s="11" customFormat="1">
+    <row r="212" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A212" s="10"/>
       <c r="B212" s="18"/>
       <c r="E212" s="30"/>
@@ -29396,7 +29396,7 @@
       <c r="BP212" s="10"/>
       <c r="BQ212" s="10"/>
     </row>
-    <row r="213" spans="1:102" s="8" customFormat="1">
+    <row r="213" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A213" s="37" t="s">
         <v>199</v>
       </c>
@@ -29761,7 +29761,7 @@
         <v>163</v>
       </c>
       <c r="L215" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M215" s="12" t="s">
         <v>165</v>
@@ -29901,7 +29901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="216" spans="1:102" s="11" customFormat="1">
+    <row r="216" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A216" s="10"/>
       <c r="B216" s="18"/>
       <c r="E216" s="30"/>
@@ -29952,7 +29952,7 @@
       <c r="BP216" s="10"/>
       <c r="BQ216" s="10"/>
     </row>
-    <row r="217" spans="1:102" s="8" customFormat="1">
+    <row r="217" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A217" s="37" t="s">
         <v>159</v>
       </c>
@@ -30317,7 +30317,7 @@
         <v>163</v>
       </c>
       <c r="L219" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M219" s="12" t="s">
         <v>165</v>
@@ -30457,7 +30457,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="220" spans="1:102" s="11" customFormat="1">
+    <row r="220" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A220" s="10"/>
       <c r="B220" s="18"/>
       <c r="E220" s="30"/>
@@ -30508,7 +30508,7 @@
       <c r="BP220" s="10"/>
       <c r="BQ220" s="10"/>
     </row>
-    <row r="221" spans="1:102" s="8" customFormat="1">
+    <row r="221" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A221" s="37" t="s">
         <v>197</v>
       </c>
@@ -30873,7 +30873,7 @@
         <v>163</v>
       </c>
       <c r="L223" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M223" s="12" t="s">
         <v>165</v>
@@ -31013,7 +31013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="224" spans="1:102" s="11" customFormat="1">
+    <row r="224" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A224" s="10"/>
       <c r="B224" s="18"/>
       <c r="E224" s="30"/>
@@ -31064,7 +31064,7 @@
       <c r="BP224" s="10"/>
       <c r="BQ224" s="10"/>
     </row>
-    <row r="225" spans="1:102" s="8" customFormat="1">
+    <row r="225" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A225" s="37" t="s">
         <v>190</v>
       </c>
@@ -31567,7 +31567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="228" spans="1:102" s="11" customFormat="1">
+    <row r="228" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A228" s="10"/>
       <c r="B228" s="18"/>
       <c r="E228" s="30"/>
@@ -31618,7 +31618,7 @@
       <c r="BP228" s="10"/>
       <c r="BQ228" s="10"/>
     </row>
-    <row r="229" spans="1:102" s="8" customFormat="1">
+    <row r="229" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A229" s="37" t="s">
         <v>239</v>
       </c>
@@ -32121,7 +32121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="232" spans="1:102" s="11" customFormat="1">
+    <row r="232" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A232" s="10"/>
       <c r="B232" s="18"/>
       <c r="E232" s="30"/>
@@ -32172,7 +32172,7 @@
       <c r="BP232" s="10"/>
       <c r="BQ232" s="10"/>
     </row>
-    <row r="233" spans="1:102" s="8" customFormat="1">
+    <row r="233" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A233" s="37" t="s">
         <v>186</v>
       </c>
@@ -32675,7 +32675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="236" spans="1:102" s="11" customFormat="1">
+    <row r="236" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A236" s="10"/>
       <c r="B236" s="18"/>
       <c r="E236" s="30"/>
@@ -32726,7 +32726,7 @@
       <c r="BP236" s="10"/>
       <c r="BQ236" s="10"/>
     </row>
-    <row r="237" spans="1:102" s="8" customFormat="1">
+    <row r="237" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A237" s="37" t="s">
         <v>205</v>
       </c>
@@ -33229,7 +33229,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="240" spans="1:102" s="11" customFormat="1">
+    <row r="240" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A240" s="10"/>
       <c r="B240" s="18"/>
       <c r="E240" s="30"/>
@@ -33280,7 +33280,7 @@
       <c r="BP240" s="10"/>
       <c r="BQ240" s="10"/>
     </row>
-    <row r="241" spans="1:102" s="26" customFormat="1">
+    <row r="241" spans="1:102" s="26" customFormat="1" ht="409.6">
       <c r="A241" s="23"/>
       <c r="B241" s="24"/>
       <c r="C241" s="23"/>
@@ -33349,7 +33349,7 @@
       <c r="BP241" s="25"/>
       <c r="BQ241" s="25"/>
     </row>
-    <row r="242" spans="1:102" s="11" customFormat="1">
+    <row r="242" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A242" s="10"/>
       <c r="B242" s="18"/>
       <c r="E242" s="30"/>
@@ -33400,7 +33400,7 @@
       <c r="BP242" s="10"/>
       <c r="BQ242" s="10"/>
     </row>
-    <row r="243" spans="1:102" s="26" customFormat="1">
+    <row r="243" spans="1:102" s="26" customFormat="1" ht="409.6">
       <c r="A243" s="23"/>
       <c r="B243" s="24"/>
       <c r="C243" s="23"/>
@@ -33469,7 +33469,7 @@
       <c r="BP243" s="25"/>
       <c r="BQ243" s="25"/>
     </row>
-    <row r="244" spans="1:102" s="26" customFormat="1">
+    <row r="244" spans="1:102" s="26" customFormat="1" ht="409.6">
       <c r="A244" s="23"/>
       <c r="B244" s="24"/>
       <c r="C244" s="23"/>
@@ -33538,7 +33538,7 @@
       <c r="BP244" s="25"/>
       <c r="BQ244" s="25"/>
     </row>
-    <row r="245" spans="1:102" s="26" customFormat="1">
+    <row r="245" spans="1:102" s="26" customFormat="1" ht="409.6">
       <c r="A245" s="23"/>
       <c r="B245" s="24"/>
       <c r="C245" s="23"/>
@@ -33607,7 +33607,7 @@
       <c r="BP245" s="25"/>
       <c r="BQ245" s="25"/>
     </row>
-    <row r="246" spans="1:102" s="26" customFormat="1">
+    <row r="246" spans="1:102" s="26" customFormat="1" ht="409.6">
       <c r="A246" s="23"/>
       <c r="B246" s="24"/>
       <c r="C246" s="23"/>
@@ -33676,7 +33676,7 @@
       <c r="BP246" s="25"/>
       <c r="BQ246" s="25"/>
     </row>
-    <row r="247" spans="1:102" s="11" customFormat="1">
+    <row r="247" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A247" s="10"/>
       <c r="B247" s="18"/>
       <c r="E247" s="10"/>
@@ -33727,7 +33727,7 @@
       <c r="BP247" s="10"/>
       <c r="BQ247" s="10"/>
     </row>
-    <row r="248" spans="1:102" s="11" customFormat="1">
+    <row r="248" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A248" s="10"/>
       <c r="B248" s="18"/>
       <c r="E248" s="10"/>
@@ -33778,7 +33778,7 @@
       <c r="BP248" s="10"/>
       <c r="BQ248" s="10"/>
     </row>
-    <row r="249" spans="1:102" s="11" customFormat="1">
+    <row r="249" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A249" s="10"/>
       <c r="B249" s="18"/>
       <c r="E249" s="10"/>
@@ -33829,7 +33829,7 @@
       <c r="BP249" s="10"/>
       <c r="BQ249" s="10"/>
     </row>
-    <row r="250" spans="1:102" s="11" customFormat="1">
+    <row r="250" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A250" s="10"/>
       <c r="B250" s="18"/>
       <c r="E250" s="10"/>
@@ -33880,7 +33880,7 @@
       <c r="BP250" s="10"/>
       <c r="BQ250" s="10"/>
     </row>
-    <row r="251" spans="1:102" s="11" customFormat="1">
+    <row r="251" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A251" s="10"/>
       <c r="B251" s="18"/>
       <c r="E251" s="10"/>
@@ -33931,7 +33931,7 @@
       <c r="BP251" s="10"/>
       <c r="BQ251" s="10"/>
     </row>
-    <row r="252" spans="1:102" s="11" customFormat="1">
+    <row r="252" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A252" s="10"/>
       <c r="B252" s="18"/>
       <c r="E252" s="10"/>

</xml_diff>

<commit_message>
latest data files as of 2018-12-17
latest data files as of 2018-12-17 - test cases pl.xlsx
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases Pl.xlsx
+++ b/src/com/data/Test Cases Pl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="23475" windowHeight="10200" tabRatio="152" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="21975" windowHeight="10200" tabRatio="152" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8058" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8058" uniqueCount="328">
   <si>
     <t>TCID</t>
   </si>
@@ -994,6 +994,12 @@
   </si>
   <si>
     <t>MsNew</t>
+  </si>
+  <si>
+    <t>1 :: N :: Y :: N :: N :: N :: N :: N :: N :: N :: N</t>
+  </si>
+  <si>
+    <t>boiler</t>
   </si>
 </sst>
 </file>
@@ -2856,8 +2862,8 @@
   <dimension ref="A1:CX252"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A135" sqref="A135"/>
+      <pane xSplit="2" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z141" sqref="Z141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -18561,7 +18567,7 @@
         <v>3</v>
       </c>
       <c r="T133" s="5" t="s">
-        <v>139</v>
+        <v>326</v>
       </c>
       <c r="U133" s="5" t="s">
         <v>311</v>
@@ -19683,7 +19689,7 @@
       <c r="X141" s="12"/>
       <c r="Y141" s="12"/>
       <c r="Z141" s="12" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="AA141" s="12" t="s">
         <v>29</v>
@@ -20479,7 +20485,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:102" s="11" customFormat="1" ht="409.6">
+    <row r="148" spans="1:102" s="11" customFormat="1">
       <c r="A148" s="10"/>
       <c r="B148" s="18"/>
       <c r="E148" s="30"/>
@@ -20530,7 +20536,7 @@
       <c r="BP148" s="10"/>
       <c r="BQ148" s="10"/>
     </row>
-    <row r="149" spans="1:102" s="8" customFormat="1" ht="409.6">
+    <row r="149" spans="1:102" s="8" customFormat="1">
       <c r="A149" s="37" t="s">
         <v>244</v>
       </c>

</xml_diff>

<commit_message>
latest data files as of 2018-12-21
latest data files as of 2018-12-21 - Test Cases Pl.xlsx
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases Pl.xlsx
+++ b/src/com/data/Test Cases Pl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="21975" windowHeight="10200" tabRatio="152" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="21615" windowHeight="6810" tabRatio="152" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8058" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8058" uniqueCount="329">
   <si>
     <t>TCID</t>
   </si>
@@ -1000,6 +1000,9 @@
   </si>
   <si>
     <t>boiler</t>
+  </si>
+  <si>
+    <t>111 :: FIRST AVENUE :: MANHATTAN :: 448 :: 28 :: Apt. MsNew</t>
   </si>
 </sst>
 </file>
@@ -2861,9 +2864,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z141" sqref="Z141"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F137" sqref="F137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -19083,7 +19086,7 @@
         <v>313</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>158</v>
+        <v>328</v>
       </c>
       <c r="G137" s="5" t="s">
         <v>162</v>
@@ -20485,7 +20488,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:102" s="11" customFormat="1">
+    <row r="148" spans="1:102" s="11" customFormat="1" ht="409.6">
       <c r="A148" s="10"/>
       <c r="B148" s="18"/>
       <c r="E148" s="30"/>
@@ -20536,7 +20539,7 @@
       <c r="BP148" s="10"/>
       <c r="BQ148" s="10"/>
     </row>
-    <row r="149" spans="1:102" s="8" customFormat="1">
+    <row r="149" spans="1:102" s="8" customFormat="1" ht="409.6">
       <c r="A149" s="37" t="s">
         <v>244</v>
       </c>

</xml_diff>